<commit_message>
HomeWork for Career Service
</commit_message>
<xml_diff>
--- a/careerServiceJobSearch_HW.xlsx
+++ b/careerServiceJobSearch_HW.xlsx
@@ -92,25 +92,26 @@
 </t>
   </si>
   <si>
-    <t>Systems Engineer</t>
-  </si>
-  <si>
-    <t>https://www.dice.com/jobs/detail/Systems-Engineer-Harris-Corporation-Clifton-NJ-07011/HARRISME1/ES20170109%26%234520681?icid=sr2-1p&amp;q=vba+macro&amp;l=NJ</t>
-  </si>
-  <si>
-    <t>Clifton, NJ</t>
-  </si>
-  <si>
-    <t>Perform the technical planning, system integration, verification and validation
-Ensure the logical and systemic conversion of customer or product requirements into total systems solutions that acknowledge technical, schedule, and cost constraints.
-Perform functional analysis, timeline analysis, detail trade studies, requirements, and allocation and interface definition studies to translate customer requirements into hardware and software specifications.
-Cost and Risk and Supportability and Effectiveness analyses for total systems (concept, design, fabrication, test, installation, operation, maintenance &amp; disposal)
-Work in a highly dynamic hardware &amp; software development and integration lab</t>
-  </si>
-  <si>
     <t xml:space="preserve">
-Gain Excel/VBA/Python , and Analytical experiences by utlilizing the skills learned from Boot Camp class.   
+Gain Analytical skills in Banking industry by utlilizing the skills learned from Boot Camp class.   
 </t>
+  </si>
+  <si>
+    <t>• Business and data analysis for the Credit Risk, Regulatory Reporting and SQL
+• Business/data analysis skills in banking
+• SQL – Data Analysis
+• Business Analyst who can perform their duties with a minimum of supervision
+• Working on Credit Risk and Regulatory reporting projects/deliverables
+• Data analysis with SQL and MS Excel</t>
+  </si>
+  <si>
+    <t>Livingston, NJ</t>
+  </si>
+  <si>
+    <t>Regulatory Reporting Business &amp; Data Analyst</t>
+  </si>
+  <si>
+    <t>https://www.dice.com/jobs/detail/Regulatory-Reporting-%26-AML-Analyst-Roles-%26%2345-Livingston%2C-NJ%28Only-W2%26%23471099%29-SoftHQ%2C-Inc.-Livingston-NJ-07039/10444954/226326?icid=sr6-1p&amp;q=Data+Analyst&amp;l=Piscataway%20Township,%20NJ</t>
   </si>
 </sst>
 </file>
@@ -195,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -226,6 +227,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -542,10 +546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3B914B-84DA-4DE6-8537-81745ABAD5B0}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -554,7 +559,7 @@
     <col min="2" max="2" width="37.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" style="7" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="78" style="1" customWidth="1"/>
     <col min="6" max="6" width="53" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -569,10 +574,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -598,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -618,24 +623,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="F9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -644,8 +654,8 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{661458F6-6D6E-4AE1-A40E-BE147123889D}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{C4CD60BB-95CB-46C9-919F-8F0198B579B8}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{59965F6F-39C3-412A-BEC3-FBBD3DFFB258}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{979B0F95-9C8E-4BAF-B202-ED9EAE94F37D}"/>
-    <hyperlink ref="A8" r:id="rId6" xr:uid="{36D8BFB0-4996-41FC-86E0-CFB0F5CE3584}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{FE4922BD-E9C0-4791-8DB7-D43C9AF2552D}"/>
+    <hyperlink ref="A9" r:id="rId6" xr:uid="{16D02C2B-F098-4577-B385-565FDF2473AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>